<commit_message>
Add BOMOutput template with new fix
</commit_message>
<xml_diff>
--- a/BOMOutputTemplate/BOMOutput.xlsx
+++ b/BOMOutputTemplate/BOMOutput.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamostler/Desktop/University/Stage 2/CSC2033 - Software Engineering Team Project/AnalysisFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamostler/Desktop/University/Stage 2/CSC2033 - Software Engineering Team Project/PriceComparisonStockChecker/BOMOutputTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79682E90-D52A-8944-9299-6FFB316E06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4AF2DB-4FB9-C345-B0A2-11E65B247554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="3340" windowWidth="28800" windowHeight="16340" xr2:uid="{24326175-27EA-C045-BCD6-24838FA9256F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="9">
   <si>
     <t>Part Number</t>
   </si>
@@ -60,14 +60,14 @@
     <t>Stock required</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +108,13 @@
       <color theme="1"/>
       <name val="Corbel (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -136,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -145,6 +152,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -450,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95C306E-1A4D-824A-A7CB-CEC7341E36AF}">
-  <dimension ref="C4:J15"/>
+  <dimension ref="C4:J327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E320" sqref="E320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,38 +501,1609 @@
       <c r="I7" t="s">
         <v>6</v>
       </c>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
       <c r="E8" s="5"/>
       <c r="F8" s="7"/>
       <c r="I8" s="6"/>
-      <c r="J8" t="s">
+      <c r="J8" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J9" t="s">
+      <c r="J9" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J10" t="s">
+      <c r="J10" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J11" t="s">
+      <c r="J11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J13" t="s">
+      <c r="J13" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J15" t="s">
+      <c r="J15" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="J16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J29" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J31" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J33" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J34" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J35" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J36" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J37" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J38" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J39" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J40" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J41" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J42" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J43" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J44" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J45" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J46" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J47" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J48" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J49" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J50" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J51" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J52" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J53" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J54" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J55" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J56" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J57" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J58" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J59" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J60" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J61" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J62" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J63" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J64" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J65" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J66" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J67" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J68" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J69" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J70" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J71" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J72" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J73" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J74" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J75" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J76" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J77" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J78" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J79" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J80" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J81" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J82" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J83" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J84" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J85" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J86" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J87" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J88" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J89" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J90" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J91" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J92" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J93" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J94" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J95" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J96" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J97" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J98" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J99" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J100" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J101" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J102" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J103" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J104" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J105" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J106" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J107" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J108" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J109" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J110" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J111" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J112" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J113" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J114" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J115" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J116" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J117" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J118" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J119" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J120" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J121" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J122" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J123" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J124" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J125" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J126" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J127" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J128" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J129" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J130" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J131" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J132" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J133" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J134" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J135" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J136" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J137" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J138" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J139" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J140" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J141" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J142" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J143" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J144" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J145" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J146" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J147" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J148" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J149" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J150" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J151" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J152" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J153" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J154" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J155" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J156" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J157" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J158" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J159" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J160" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J161" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J162" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J163" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J164" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J165" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J166" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J167" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J168" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J169" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J170" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J171" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J172" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J173" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J174" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J175" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J176" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J177" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J178" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J179" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J180" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J181" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J182" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J183" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J184" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J185" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J186" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J187" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J188" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="189" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J189" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J190" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J191" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J192" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J193" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J194" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J195" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J196" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J197" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J198" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J199" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J200" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="201" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J201" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="202" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J202" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J203" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="204" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J204" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="205" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J205" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J206" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J207" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J208" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J209" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J210" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J211" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J212" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J213" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J214" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J215" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J216" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J217" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J218" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J219" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J220" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J221" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J222" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J223" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J224" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J225" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J226" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J227" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J228" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J229" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J230" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J231" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J232" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J233" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J234" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J235" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J236" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J237" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J238" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J239" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J240" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J241" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J242" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J243" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J244" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J245" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J246" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J247" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J248" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J249" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J250" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J251" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J252" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J253" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J254" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J255" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J256" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J257" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J258" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J259" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J260" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J261" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J262" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J263" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J264" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="265" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J265" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="266" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J266" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J267" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J268" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J269" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J270" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="271" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J271" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J272" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="273" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J273" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J274" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J275" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J276" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="277" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J277" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="278" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J278" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="279" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J279" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J280" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J281" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J282" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J283" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J284" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J285" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J286" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J287" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J288" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J289" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J290" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J291" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J292" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="293" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J293" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="294" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J294" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="295" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J295" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="296" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J296" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J297" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J298" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="299" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J299" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J300" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J301" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J302" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J303" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J304" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="305" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J305" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="306" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J306" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="307" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J307" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="308" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J308" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="309" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J309" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="310" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J310" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="311" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J311" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="312" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J312" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="313" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J313" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="314" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J314" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J315" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="316" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J316" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="317" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J317" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="318" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J318" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="319" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J319" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J320" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="321" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J321" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="322" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J322" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="323" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J323" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="324" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J324" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="325" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J325" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="326" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J326" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="327" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J327" s="8" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BOM Output files. change font and size of text
</commit_message>
<xml_diff>
--- a/BOMOutputTemplate/BOMOutput.xlsx
+++ b/BOMOutputTemplate/BOMOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamostler/Desktop/University/Stage 2/CSC2033 - Software Engineering Team Project/PriceComparisonStockChecker/BOMOutputTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4AF2DB-4FB9-C345-B0A2-11E65B247554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66110696-C6A4-0B4D-8974-3ABB10B66ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="3340" windowWidth="28800" windowHeight="16340" xr2:uid="{24326175-27EA-C045-BCD6-24838FA9256F}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Part Number</t>
   </si>
   <si>
-    <t>Bill of Materials - Search Results</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   <si>
     <t>blank</t>
   </si>
+  <si>
+    <t xml:space="preserve">                  Bill of Materials - Search Results</t>
+  </si>
 </sst>
 </file>
 
@@ -71,7 +71,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Corbel"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +79,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Corbel"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,12 +111,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Corbel"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +129,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -138,12 +144,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -153,6 +185,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -203,15 +238,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>7055</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>197555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1257120</xdr:colOff>
+      <xdr:colOff>706786</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>43744</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -226,7 +261,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -234,14 +269,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="2487"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1739900" y="596900"/>
-          <a:ext cx="3517720" cy="876300"/>
+          <a:off x="1912055" y="606777"/>
+          <a:ext cx="3430231" cy="880534"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -310,16 +344,76 @@
         <a:srgbClr val="8C8C8C"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Headlines">
+    <a:fontScheme name="Arial">
       <a:majorFont>
-        <a:latin typeface="Century Schoolbook" panose="02040604050505020304"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Corbel" panose="020B0503020204020204"/>
+        <a:latin typeface="Arial" panose="020B0604020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="굴림"/>
+        <a:font script="Hans" typeface="黑体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Headlines">
@@ -458,48 +552,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95C306E-1A4D-824A-A7CB-CEC7341E36AF}">
-  <dimension ref="C4:J327"/>
+  <dimension ref="C2:J327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E320" sqref="E320"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="9" width="20.83203125" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="9"/>
+    </row>
     <row r="4" spans="3:10" ht="35" x14ac:dyDescent="0.45">
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="3:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
       </c>
       <c r="J7" s="8"/>
     </row>
@@ -509,1602 +611,1602 @@
       <c r="F8" s="7"/>
       <c r="I8" s="6"/>
       <c r="J8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J9" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J10" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J14" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J15" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J16" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J18" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J19" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J20" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J21" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J22" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J23" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J24" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J25" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J26" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J27" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J28" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J29" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J30" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J31" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J32" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J33" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J34" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J35" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J36" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J37" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J38" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J39" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J40" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J41" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J42" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J43" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J44" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J45" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J46" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J47" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J48" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J49" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J50" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J51" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J52" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J53" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J54" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J55" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J56" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J57" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J58" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J59" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J60" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J61" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J62" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J63" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J64" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J65" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J66" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J67" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J68" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J69" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J70" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J71" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J72" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J73" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J74" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J75" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J76" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J77" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J78" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J79" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J80" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J81" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J82" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J83" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J84" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J85" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J86" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J87" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J88" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J89" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J90" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J91" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J92" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J93" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J94" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J95" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J96" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J97" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J98" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J99" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J100" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J101" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J102" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J103" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J104" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J105" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J106" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J107" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J108" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J109" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J110" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J111" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J112" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J113" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J114" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J115" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J116" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J117" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J118" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J119" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J120" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J121" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J122" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J123" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J124" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J125" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J126" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J127" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J128" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="129" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J129" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J130" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J131" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J132" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J133" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J134" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J135" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="136" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J136" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J137" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J138" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J139" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J140" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="141" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J141" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J142" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="143" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J143" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J144" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J145" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J146" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J147" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J148" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="149" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J149" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J150" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="151" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J151" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="152" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J152" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="153" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J153" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="154" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J154" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="155" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J155" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="156" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J156" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="157" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J157" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="158" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J158" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="159" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J159" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="160" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J160" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J161" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J162" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="163" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J163" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J164" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="165" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J165" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J166" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J167" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J168" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J169" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J170" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J171" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="172" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J172" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="173" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J173" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J174" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J175" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J176" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="177" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J177" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J178" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J179" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J180" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="181" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J181" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J182" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="183" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J183" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="184" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J184" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="185" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J185" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="186" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J186" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="187" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J187" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="188" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J188" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="189" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J189" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="190" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J190" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J191" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="192" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J192" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J193" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="194" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J194" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="195" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J195" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="196" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J196" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J197" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="198" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J198" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="199" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J199" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="200" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J200" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J201" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="202" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J202" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="203" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J203" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J204" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="205" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J205" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="206" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J206" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="207" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J207" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="208" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J208" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J209" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J210" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="211" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J211" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="212" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J212" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="213" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J213" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="214" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J214" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="215" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J215" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="216" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J216" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="217" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J217" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="218" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J218" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="219" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J219" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="220" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J220" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="221" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J221" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J222" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="223" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J223" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="224" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J224" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="225" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J225" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="226" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J226" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="227" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J227" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="228" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J228" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="229" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J229" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="230" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J230" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="231" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J231" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="232" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J232" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="233" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J233" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="234" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J234" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="235" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J235" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J236" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="237" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J237" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="238" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J238" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="239" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J239" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="240" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J240" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="241" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J241" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="242" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J242" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="243" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J243" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="244" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J244" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="245" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J245" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J246" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="247" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J247" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="248" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J248" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="249" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J249" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="250" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J250" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="251" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J251" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="252" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J252" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="253" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J253" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="254" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J254" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="255" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J255" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="256" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J256" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="257" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J257" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="258" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J258" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="259" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J259" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="260" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J260" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="261" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J261" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="262" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J262" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="263" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J263" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="264" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J264" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="265" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J265" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="266" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J266" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="267" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J267" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="268" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J268" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="269" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J269" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="270" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J270" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="271" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J271" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="272" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J272" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="273" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J273" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="274" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J274" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="275" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J275" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="276" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J276" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="277" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J277" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="278" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J278" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="279" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J279" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="280" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J280" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="281" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J281" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="282" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J282" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="283" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J283" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="284" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J284" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="285" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J285" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="286" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J286" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="287" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J287" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="288" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J288" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="289" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J289" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="290" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J290" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="291" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J291" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="292" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J292" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="293" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J293" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="294" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J294" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="295" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J295" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="296" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J296" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="297" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J297" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="298" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J298" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="299" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J299" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="300" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J300" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="301" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J301" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="302" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J302" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="303" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J303" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="304" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J304" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="305" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J305" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="306" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J306" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="307" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J307" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="308" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J308" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="309" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J309" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="310" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J310" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="311" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J311" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="312" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J312" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="313" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J313" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="314" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J314" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="315" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J315" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="316" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J316" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="317" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J317" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="318" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J318" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="319" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J319" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="320" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J320" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="321" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J321" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="322" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J322" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="323" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J323" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="324" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J324" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="325" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J325" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="326" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J326" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="327" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J327" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>